<commit_message>
UPDATE robot.db | prototipo 1 | falta legacy
</commit_message>
<xml_diff>
--- a/resources/articulos_disponibles_ventas.xlsx
+++ b/resources/articulos_disponibles_ventas.xlsx
@@ -34,7 +34,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,17 +412,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="10.88671875" customWidth="1" min="1" max="1"/>
-    <col width="19.6640625" customWidth="1" min="2" max="6"/>
-    <col width="17.77734375" customWidth="1" min="7" max="7"/>
+    <col width="13.77734375" customWidth="1" min="1" max="1"/>
+    <col width="17.88671875" customWidth="1" min="2" max="6"/>
+    <col width="11.88671875" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,25 +463,137 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>chocolate</t>
+          <t>Laptop Lenovo IdeaPad 3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>golosinas</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>750000.0</t>
         </is>
       </c>
       <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Apple iPad Air</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>550000.0</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Telefono Movil</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>300000.0</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>10</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>milka</t>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Google Pixel 6</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Telefono Movil</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>700000.0</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>HP Spectre x360</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1300000.0</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>HP</t>
         </is>
       </c>
     </row>

</xml_diff>